<commit_message>
adjusted the cost and the plots in the exploration.
</commit_message>
<xml_diff>
--- a/data/stones.xlsx
+++ b/data/stones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauernd\Documents\R\workspace\lap\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EE18FB-580B-4D1D-AECD-554FAB94161E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A02D2E-A844-45F8-B59B-3259E8E45BC1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="630" windowWidth="18705" windowHeight="10290" xr2:uid="{6B4F78AC-19D9-4168-B59C-6175042E22EC}"/>
+    <workbookView xWindow="2475" yWindow="1410" windowWidth="18900" windowHeight="11055" xr2:uid="{6B4F78AC-19D9-4168-B59C-6175042E22EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,7 +428,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -439,7 +439,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -450,7 +450,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -461,7 +461,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -472,7 +472,7 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -483,7 +483,7 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -494,7 +494,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -505,7 +505,7 @@
         <v>2</v>
       </c>
       <c r="C9">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -516,7 +516,7 @@
         <v>2</v>
       </c>
       <c r="C10">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -527,7 +527,7 @@
         <v>2</v>
       </c>
       <c r="C11">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
         <v>2</v>
       </c>
       <c r="C12">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -549,7 +549,7 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -560,7 +560,7 @@
         <v>2</v>
       </c>
       <c r="C14">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -571,7 +571,7 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -582,7 +582,7 @@
         <v>2</v>
       </c>
       <c r="C16">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
         <v>2</v>
       </c>
       <c r="C17">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -604,7 +604,7 @@
         <v>2</v>
       </c>
       <c r="C18">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -615,7 +615,7 @@
         <v>2</v>
       </c>
       <c r="C19">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -626,7 +626,7 @@
         <v>2</v>
       </c>
       <c r="C20">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -637,7 +637,7 @@
         <v>2</v>
       </c>
       <c r="C21">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -648,7 +648,7 @@
         <v>2</v>
       </c>
       <c r="C22">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -659,7 +659,7 @@
         <v>2</v>
       </c>
       <c r="C23">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -670,7 +670,7 @@
         <v>2</v>
       </c>
       <c r="C24">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -681,7 +681,7 @@
         <v>2</v>
       </c>
       <c r="C25">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -692,7 +692,7 @@
         <v>2</v>
       </c>
       <c r="C26">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -703,7 +703,7 @@
         <v>2</v>
       </c>
       <c r="C27">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -714,7 +714,7 @@
         <v>2</v>
       </c>
       <c r="C28">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -725,7 +725,7 @@
         <v>2</v>
       </c>
       <c r="C29">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -736,7 +736,7 @@
         <v>2</v>
       </c>
       <c r="C30">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -747,7 +747,7 @@
         <v>2</v>
       </c>
       <c r="C31">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -758,7 +758,7 @@
         <v>2</v>
       </c>
       <c r="C32">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -769,7 +769,7 @@
         <v>2</v>
       </c>
       <c r="C33">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -780,7 +780,7 @@
         <v>2</v>
       </c>
       <c r="C34">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -791,7 +791,7 @@
         <v>2</v>
       </c>
       <c r="C35">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -802,7 +802,7 @@
         <v>2</v>
       </c>
       <c r="C36">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -813,7 +813,7 @@
         <v>2</v>
       </c>
       <c r="C37">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -824,7 +824,7 @@
         <v>2</v>
       </c>
       <c r="C38">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -835,7 +835,7 @@
         <v>2</v>
       </c>
       <c r="C39">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -846,7 +846,7 @@
         <v>2</v>
       </c>
       <c r="C40">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -857,7 +857,7 @@
         <v>2</v>
       </c>
       <c r="C41">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -868,7 +868,7 @@
         <v>2</v>
       </c>
       <c r="C42">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -879,7 +879,7 @@
         <v>2</v>
       </c>
       <c r="C43">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -890,7 +890,7 @@
         <v>2</v>
       </c>
       <c r="C44">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -901,7 +901,7 @@
         <v>2</v>
       </c>
       <c r="C45">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -912,7 +912,7 @@
         <v>2</v>
       </c>
       <c r="C46">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -923,7 +923,7 @@
         <v>2</v>
       </c>
       <c r="C47">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -934,7 +934,7 @@
         <v>2</v>
       </c>
       <c r="C48">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -945,7 +945,7 @@
         <v>2</v>
       </c>
       <c r="C49">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -956,7 +956,7 @@
         <v>2</v>
       </c>
       <c r="C50">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -967,7 +967,7 @@
         <v>2</v>
       </c>
       <c r="C51">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -978,7 +978,7 @@
         <v>2</v>
       </c>
       <c r="C52">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -989,7 +989,7 @@
         <v>2</v>
       </c>
       <c r="C53">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1000,7 +1000,7 @@
         <v>2</v>
       </c>
       <c r="C54">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1011,7 +1011,7 @@
         <v>2</v>
       </c>
       <c r="C55">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1022,7 +1022,7 @@
         <v>2</v>
       </c>
       <c r="C56">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1033,7 +1033,7 @@
         <v>2</v>
       </c>
       <c r="C57">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1044,7 +1044,7 @@
         <v>2</v>
       </c>
       <c r="C58">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1055,7 +1055,7 @@
         <v>2</v>
       </c>
       <c r="C59">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1066,7 +1066,7 @@
         <v>2</v>
       </c>
       <c r="C60">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1077,7 +1077,7 @@
         <v>2</v>
       </c>
       <c r="C61">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1088,7 +1088,7 @@
         <v>2</v>
       </c>
       <c r="C62">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1099,7 +1099,7 @@
         <v>2</v>
       </c>
       <c r="C63">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1110,7 +1110,7 @@
         <v>2</v>
       </c>
       <c r="C64">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1121,7 +1121,7 @@
         <v>2</v>
       </c>
       <c r="C65">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1132,7 +1132,7 @@
         <v>2</v>
       </c>
       <c r="C66">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1143,7 +1143,7 @@
         <v>2</v>
       </c>
       <c r="C67">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1154,7 +1154,7 @@
         <v>2</v>
       </c>
       <c r="C68">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1165,7 +1165,7 @@
         <v>2</v>
       </c>
       <c r="C69">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1176,7 +1176,7 @@
         <v>2</v>
       </c>
       <c r="C70">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1187,7 +1187,7 @@
         <v>2</v>
       </c>
       <c r="C71">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1198,7 +1198,7 @@
         <v>2</v>
       </c>
       <c r="C72">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1209,7 +1209,7 @@
         <v>2</v>
       </c>
       <c r="C73">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1220,7 +1220,7 @@
         <v>2</v>
       </c>
       <c r="C74">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1231,7 +1231,7 @@
         <v>2</v>
       </c>
       <c r="C75">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1242,7 +1242,7 @@
         <v>2</v>
       </c>
       <c r="C76">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1253,7 +1253,7 @@
         <v>2</v>
       </c>
       <c r="C77">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1264,7 +1264,7 @@
         <v>2</v>
       </c>
       <c r="C78">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1275,7 +1275,7 @@
         <v>2</v>
       </c>
       <c r="C79">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1286,7 +1286,7 @@
         <v>2</v>
       </c>
       <c r="C80">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1297,7 +1297,7 @@
         <v>2</v>
       </c>
       <c r="C81">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -1308,7 +1308,7 @@
         <v>2</v>
       </c>
       <c r="C82">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1319,7 +1319,7 @@
         <v>2</v>
       </c>
       <c r="C83">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -1330,7 +1330,7 @@
         <v>2</v>
       </c>
       <c r="C84">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -1341,7 +1341,7 @@
         <v>2</v>
       </c>
       <c r="C85">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1352,7 +1352,7 @@
         <v>2</v>
       </c>
       <c r="C86">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1363,7 +1363,7 @@
         <v>2</v>
       </c>
       <c r="C87">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -1374,7 +1374,7 @@
         <v>2</v>
       </c>
       <c r="C88">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -1385,7 +1385,7 @@
         <v>2</v>
       </c>
       <c r="C89">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -1396,7 +1396,7 @@
         <v>2</v>
       </c>
       <c r="C90">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -1407,7 +1407,7 @@
         <v>2</v>
       </c>
       <c r="C91">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -1418,7 +1418,7 @@
         <v>2</v>
       </c>
       <c r="C92">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -1429,7 +1429,7 @@
         <v>3</v>
       </c>
       <c r="C93">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -1440,7 +1440,7 @@
         <v>3</v>
       </c>
       <c r="C94">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -1451,7 +1451,7 @@
         <v>3</v>
       </c>
       <c r="C95">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -1462,7 +1462,7 @@
         <v>3</v>
       </c>
       <c r="C96">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -1473,7 +1473,7 @@
         <v>3</v>
       </c>
       <c r="C97">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -1484,7 +1484,7 @@
         <v>3</v>
       </c>
       <c r="C98">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -1495,7 +1495,7 @@
         <v>3</v>
       </c>
       <c r="C99">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -1506,7 +1506,7 @@
         <v>3</v>
       </c>
       <c r="C100">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -1517,7 +1517,7 @@
         <v>3</v>
       </c>
       <c r="C101">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -1528,7 +1528,7 @@
         <v>3</v>
       </c>
       <c r="C102">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -1539,7 +1539,7 @@
         <v>3</v>
       </c>
       <c r="C103">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -1550,7 +1550,7 @@
         <v>3</v>
       </c>
       <c r="C104">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -1561,7 +1561,7 @@
         <v>3</v>
       </c>
       <c r="C105">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -1572,7 +1572,7 @@
         <v>3</v>
       </c>
       <c r="C106">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -1583,7 +1583,7 @@
         <v>3</v>
       </c>
       <c r="C107">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -1594,7 +1594,7 @@
         <v>3</v>
       </c>
       <c r="C108">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -1605,7 +1605,7 @@
         <v>3</v>
       </c>
       <c r="C109">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -1616,7 +1616,7 @@
         <v>3</v>
       </c>
       <c r="C110">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -1627,7 +1627,7 @@
         <v>3</v>
       </c>
       <c r="C111">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -1638,7 +1638,7 @@
         <v>3</v>
       </c>
       <c r="C112">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -1649,7 +1649,7 @@
         <v>3</v>
       </c>
       <c r="C113">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -1660,7 +1660,7 @@
         <v>3</v>
       </c>
       <c r="C114">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -1671,7 +1671,7 @@
         <v>3</v>
       </c>
       <c r="C115">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -1682,7 +1682,7 @@
         <v>3</v>
       </c>
       <c r="C116">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -1693,7 +1693,7 @@
         <v>3</v>
       </c>
       <c r="C117">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -1704,7 +1704,7 @@
         <v>3</v>
       </c>
       <c r="C118">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -1715,7 +1715,7 @@
         <v>3</v>
       </c>
       <c r="C119">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -1726,7 +1726,7 @@
         <v>3</v>
       </c>
       <c r="C120">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -1737,7 +1737,7 @@
         <v>3</v>
       </c>
       <c r="C121">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -1748,7 +1748,7 @@
         <v>3</v>
       </c>
       <c r="C122">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -1759,7 +1759,7 @@
         <v>3</v>
       </c>
       <c r="C123">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -1770,7 +1770,7 @@
         <v>3</v>
       </c>
       <c r="C124">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -1781,7 +1781,7 @@
         <v>3</v>
       </c>
       <c r="C125">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -1792,7 +1792,7 @@
         <v>3</v>
       </c>
       <c r="C126">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -1803,7 +1803,7 @@
         <v>3</v>
       </c>
       <c r="C127">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -1814,7 +1814,7 @@
         <v>3</v>
       </c>
       <c r="C128">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -1825,7 +1825,7 @@
         <v>3</v>
       </c>
       <c r="C129">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -1836,7 +1836,7 @@
         <v>3</v>
       </c>
       <c r="C130">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -1847,7 +1847,7 @@
         <v>3</v>
       </c>
       <c r="C131">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -1858,7 +1858,7 @@
         <v>3</v>
       </c>
       <c r="C132">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -1869,7 +1869,7 @@
         <v>3</v>
       </c>
       <c r="C133">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -1880,7 +1880,7 @@
         <v>3</v>
       </c>
       <c r="C134">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -1891,7 +1891,7 @@
         <v>3</v>
       </c>
       <c r="C135">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -1902,7 +1902,7 @@
         <v>3</v>
       </c>
       <c r="C136">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -1913,7 +1913,7 @@
         <v>3</v>
       </c>
       <c r="C137">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -1924,7 +1924,7 @@
         <v>3</v>
       </c>
       <c r="C138">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -1935,7 +1935,7 @@
         <v>3</v>
       </c>
       <c r="C139">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -1946,7 +1946,7 @@
         <v>3</v>
       </c>
       <c r="C140">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -1957,7 +1957,7 @@
         <v>3</v>
       </c>
       <c r="C141">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -1968,7 +1968,7 @@
         <v>3</v>
       </c>
       <c r="C142">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -1979,7 +1979,7 @@
         <v>3</v>
       </c>
       <c r="C143">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -1990,7 +1990,7 @@
         <v>3</v>
       </c>
       <c r="C144">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -2001,7 +2001,7 @@
         <v>3</v>
       </c>
       <c r="C145">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -2012,7 +2012,7 @@
         <v>3</v>
       </c>
       <c r="C146">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -2023,7 +2023,7 @@
         <v>3</v>
       </c>
       <c r="C147">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -2034,7 +2034,7 @@
         <v>3</v>
       </c>
       <c r="C148">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -2045,7 +2045,7 @@
         <v>3</v>
       </c>
       <c r="C149">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -2056,7 +2056,7 @@
         <v>3</v>
       </c>
       <c r="C150">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -2067,7 +2067,7 @@
         <v>3</v>
       </c>
       <c r="C151">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -2078,7 +2078,7 @@
         <v>3</v>
       </c>
       <c r="C152">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -2089,7 +2089,7 @@
         <v>3</v>
       </c>
       <c r="C153">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -2100,7 +2100,7 @@
         <v>3</v>
       </c>
       <c r="C154">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -2111,7 +2111,7 @@
         <v>3</v>
       </c>
       <c r="C155">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -2122,7 +2122,7 @@
         <v>3</v>
       </c>
       <c r="C156">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -2133,7 +2133,7 @@
         <v>3</v>
       </c>
       <c r="C157">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -2144,7 +2144,7 @@
         <v>3</v>
       </c>
       <c r="C158">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -2155,7 +2155,7 @@
         <v>3</v>
       </c>
       <c r="C159">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -2166,7 +2166,7 @@
         <v>3</v>
       </c>
       <c r="C160">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -2177,7 +2177,7 @@
         <v>3</v>
       </c>
       <c r="C161">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -2188,7 +2188,7 @@
         <v>3</v>
       </c>
       <c r="C162">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -2199,7 +2199,7 @@
         <v>3</v>
       </c>
       <c r="C163">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -2210,7 +2210,7 @@
         <v>3</v>
       </c>
       <c r="C164">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -2221,7 +2221,7 @@
         <v>3</v>
       </c>
       <c r="C165">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -2232,7 +2232,7 @@
         <v>3</v>
       </c>
       <c r="C166">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -2243,7 +2243,7 @@
         <v>3</v>
       </c>
       <c r="C167">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -2254,7 +2254,7 @@
         <v>3</v>
       </c>
       <c r="C168">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -2265,7 +2265,7 @@
         <v>3</v>
       </c>
       <c r="C169">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -2276,7 +2276,7 @@
         <v>3</v>
       </c>
       <c r="C170">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -2287,7 +2287,7 @@
         <v>3</v>
       </c>
       <c r="C171">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -2298,7 +2298,7 @@
         <v>3</v>
       </c>
       <c r="C172">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -2309,7 +2309,7 @@
         <v>3</v>
       </c>
       <c r="C173">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -2320,7 +2320,7 @@
         <v>3</v>
       </c>
       <c r="C174">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -2331,7 +2331,7 @@
         <v>3</v>
       </c>
       <c r="C175">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -2342,7 +2342,7 @@
         <v>3</v>
       </c>
       <c r="C176">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -2353,7 +2353,7 @@
         <v>3</v>
       </c>
       <c r="C177">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -2364,7 +2364,7 @@
         <v>3</v>
       </c>
       <c r="C178">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -2375,7 +2375,7 @@
         <v>3</v>
       </c>
       <c r="C179">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -2386,7 +2386,7 @@
         <v>3</v>
       </c>
       <c r="C180">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -2397,7 +2397,7 @@
         <v>3</v>
       </c>
       <c r="C181">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -2408,7 +2408,7 @@
         <v>3</v>
       </c>
       <c r="C182">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -2419,7 +2419,7 @@
         <v>3</v>
       </c>
       <c r="C183">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -2430,7 +2430,7 @@
         <v>3</v>
       </c>
       <c r="C184">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -2441,7 +2441,7 @@
         <v>3</v>
       </c>
       <c r="C185">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -2452,7 +2452,7 @@
         <v>3</v>
       </c>
       <c r="C186">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -2463,7 +2463,7 @@
         <v>3</v>
       </c>
       <c r="C187">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -2474,7 +2474,7 @@
         <v>3</v>
       </c>
       <c r="C188">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -2485,7 +2485,7 @@
         <v>3</v>
       </c>
       <c r="C189">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -2496,7 +2496,7 @@
         <v>3</v>
       </c>
       <c r="C190">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -2507,7 +2507,7 @@
         <v>3</v>
       </c>
       <c r="C191">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -2518,7 +2518,7 @@
         <v>3</v>
       </c>
       <c r="C192">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -2529,7 +2529,7 @@
         <v>3</v>
       </c>
       <c r="C193">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -2540,7 +2540,7 @@
         <v>3</v>
       </c>
       <c r="C194">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -2551,7 +2551,7 @@
         <v>3</v>
       </c>
       <c r="C195">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -2562,7 +2562,7 @@
         <v>3</v>
       </c>
       <c r="C196">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -2573,7 +2573,7 @@
         <v>3</v>
       </c>
       <c r="C197">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -2584,7 +2584,7 @@
         <v>3</v>
       </c>
       <c r="C198">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -2595,7 +2595,7 @@
         <v>3</v>
       </c>
       <c r="C199">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -2606,7 +2606,7 @@
         <v>3</v>
       </c>
       <c r="C200">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -2617,7 +2617,7 @@
         <v>3</v>
       </c>
       <c r="C201">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -2628,7 +2628,7 @@
         <v>3</v>
       </c>
       <c r="C202">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -2639,7 +2639,7 @@
         <v>3</v>
       </c>
       <c r="C203">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -2650,7 +2650,7 @@
         <v>3</v>
       </c>
       <c r="C204">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -2661,7 +2661,7 @@
         <v>3</v>
       </c>
       <c r="C205">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -2672,7 +2672,7 @@
         <v>3</v>
       </c>
       <c r="C206">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -2683,7 +2683,7 @@
         <v>3</v>
       </c>
       <c r="C207">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -2694,7 +2694,7 @@
         <v>3</v>
       </c>
       <c r="C208">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -2705,7 +2705,7 @@
         <v>3</v>
       </c>
       <c r="C209">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -2716,7 +2716,7 @@
         <v>3</v>
       </c>
       <c r="C210">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -2727,7 +2727,7 @@
         <v>3</v>
       </c>
       <c r="C211">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
@@ -2738,7 +2738,7 @@
         <v>3</v>
       </c>
       <c r="C212">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
@@ -2749,7 +2749,7 @@
         <v>3</v>
       </c>
       <c r="C213">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -2760,7 +2760,7 @@
         <v>3</v>
       </c>
       <c r="C214">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
@@ -2771,7 +2771,7 @@
         <v>3</v>
       </c>
       <c r="C215">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
@@ -2782,7 +2782,7 @@
         <v>3</v>
       </c>
       <c r="C216">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
@@ -2793,7 +2793,7 @@
         <v>3</v>
       </c>
       <c r="C217">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
@@ -2804,7 +2804,7 @@
         <v>3</v>
       </c>
       <c r="C218">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -2815,7 +2815,7 @@
         <v>3</v>
       </c>
       <c r="C219">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
@@ -2826,7 +2826,7 @@
         <v>3</v>
       </c>
       <c r="C220">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
@@ -2837,7 +2837,7 @@
         <v>3</v>
       </c>
       <c r="C221">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
@@ -2848,7 +2848,7 @@
         <v>3</v>
       </c>
       <c r="C222">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
@@ -2859,7 +2859,7 @@
         <v>3</v>
       </c>
       <c r="C223">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
@@ -2870,7 +2870,7 @@
         <v>3</v>
       </c>
       <c r="C224">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -2881,7 +2881,7 @@
         <v>3</v>
       </c>
       <c r="C225">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -2892,7 +2892,7 @@
         <v>3</v>
       </c>
       <c r="C226">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
@@ -2903,7 +2903,7 @@
         <v>3</v>
       </c>
       <c r="C227">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -2914,7 +2914,7 @@
         <v>3</v>
       </c>
       <c r="C228">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -2925,7 +2925,7 @@
         <v>3</v>
       </c>
       <c r="C229">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
@@ -2936,7 +2936,7 @@
         <v>3</v>
       </c>
       <c r="C230">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -2947,7 +2947,7 @@
         <v>3</v>
       </c>
       <c r="C231">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -2958,7 +2958,7 @@
         <v>3</v>
       </c>
       <c r="C232">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -2969,7 +2969,7 @@
         <v>3</v>
       </c>
       <c r="C233">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -2980,7 +2980,7 @@
         <v>3</v>
       </c>
       <c r="C234">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -2991,7 +2991,7 @@
         <v>3</v>
       </c>
       <c r="C235">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -3002,7 +3002,7 @@
         <v>3</v>
       </c>
       <c r="C236">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -3013,7 +3013,7 @@
         <v>3</v>
       </c>
       <c r="C237">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -3024,7 +3024,7 @@
         <v>3</v>
       </c>
       <c r="C238">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -3035,7 +3035,7 @@
         <v>3</v>
       </c>
       <c r="C239">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
@@ -3046,7 +3046,7 @@
         <v>3</v>
       </c>
       <c r="C240">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -3057,7 +3057,7 @@
         <v>3</v>
       </c>
       <c r="C241">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
@@ -3068,7 +3068,7 @@
         <v>3</v>
       </c>
       <c r="C242">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
@@ -3079,7 +3079,7 @@
         <v>3</v>
       </c>
       <c r="C243">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
@@ -3090,7 +3090,7 @@
         <v>3</v>
       </c>
       <c r="C244">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -3101,7 +3101,7 @@
         <v>3</v>
       </c>
       <c r="C245">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -3112,7 +3112,7 @@
         <v>3</v>
       </c>
       <c r="C246">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
@@ -3123,7 +3123,7 @@
         <v>3</v>
       </c>
       <c r="C247">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
@@ -3134,7 +3134,7 @@
         <v>3</v>
       </c>
       <c r="C248">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
@@ -3145,7 +3145,7 @@
         <v>3</v>
       </c>
       <c r="C249">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
@@ -3156,7 +3156,7 @@
         <v>3</v>
       </c>
       <c r="C250">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
@@ -3167,7 +3167,7 @@
         <v>3</v>
       </c>
       <c r="C251">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
@@ -3178,7 +3178,7 @@
         <v>3</v>
       </c>
       <c r="C252">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
@@ -3189,7 +3189,7 @@
         <v>3</v>
       </c>
       <c r="C253">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
@@ -3200,7 +3200,7 @@
         <v>3</v>
       </c>
       <c r="C254">
-        <v>3.3000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
@@ -3211,7 +3211,7 @@
         <v>5</v>
       </c>
       <c r="C255">
-        <v>3.3000000000000002E-2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
@@ -3222,7 +3222,7 @@
         <v>5</v>
       </c>
       <c r="C256">
-        <v>3.3000000000000002E-2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
@@ -3233,7 +3233,7 @@
         <v>5</v>
       </c>
       <c r="C257">
-        <v>3.3000000000000002E-2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
@@ -3244,7 +3244,7 @@
         <v>5</v>
       </c>
       <c r="C258">
-        <v>3.3000000000000002E-2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
@@ -3255,7 +3255,7 @@
         <v>5</v>
       </c>
       <c r="C259">
-        <v>3.3000000000000002E-2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
@@ -3266,7 +3266,7 @@
         <v>5</v>
       </c>
       <c r="C260">
-        <v>3.3000000000000002E-2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -3277,7 +3277,7 @@
         <v>5</v>
       </c>
       <c r="C261">
-        <v>3.3000000000000002E-2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -3288,7 +3288,7 @@
         <v>5</v>
       </c>
       <c r="C262">
-        <v>3.3000000000000002E-2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -3299,7 +3299,7 @@
         <v>5</v>
       </c>
       <c r="C263">
-        <v>3.3000000000000002E-2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
@@ -3310,7 +3310,7 @@
         <v>5</v>
       </c>
       <c r="C264">
-        <v>3.3000000000000002E-2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -3321,7 +3321,7 @@
         <v>5</v>
       </c>
       <c r="C265">
-        <v>3.3000000000000002E-2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -3332,7 +3332,7 @@
         <v>5</v>
       </c>
       <c r="C266">
-        <v>3.3000000000000002E-2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
@@ -3343,7 +3343,7 @@
         <v>5</v>
       </c>
       <c r="C267">
-        <v>3.3000000000000002E-2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -3354,7 +3354,7 @@
         <v>5</v>
       </c>
       <c r="C268">
-        <v>3.3000000000000002E-2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -3365,7 +3365,7 @@
         <v>6</v>
       </c>
       <c r="C269">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
@@ -3376,7 +3376,7 @@
         <v>6</v>
       </c>
       <c r="C270">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -3387,7 +3387,7 @@
         <v>6</v>
       </c>
       <c r="C271">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
@@ -3398,7 +3398,7 @@
         <v>6</v>
       </c>
       <c r="C272">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -3409,7 +3409,7 @@
         <v>6</v>
       </c>
       <c r="C273">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -3420,7 +3420,7 @@
         <v>6</v>
       </c>
       <c r="C274">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -3431,7 +3431,7 @@
         <v>6</v>
       </c>
       <c r="C275">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
@@ -3442,7 +3442,7 @@
         <v>6</v>
       </c>
       <c r="C276">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -3453,7 +3453,7 @@
         <v>6</v>
       </c>
       <c r="C277">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -3464,7 +3464,7 @@
         <v>6</v>
       </c>
       <c r="C278">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -3475,7 +3475,7 @@
         <v>6</v>
       </c>
       <c r="C279">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -3486,7 +3486,7 @@
         <v>6</v>
       </c>
       <c r="C280">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -3497,7 +3497,7 @@
         <v>6</v>
       </c>
       <c r="C281">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
@@ -3508,7 +3508,7 @@
         <v>6</v>
       </c>
       <c r="C282">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
@@ -3519,7 +3519,7 @@
         <v>6</v>
       </c>
       <c r="C283">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -3530,7 +3530,7 @@
         <v>6</v>
       </c>
       <c r="C284">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
@@ -3541,7 +3541,7 @@
         <v>6</v>
       </c>
       <c r="C285">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -3552,7 +3552,7 @@
         <v>6</v>
       </c>
       <c r="C286">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -3563,7 +3563,7 @@
         <v>6</v>
       </c>
       <c r="C287">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
@@ -3574,7 +3574,7 @@
         <v>6</v>
       </c>
       <c r="C288">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
@@ -3585,7 +3585,7 @@
         <v>6</v>
       </c>
       <c r="C289">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
@@ -3596,7 +3596,7 @@
         <v>6</v>
       </c>
       <c r="C290">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
@@ -3607,7 +3607,7 @@
         <v>6</v>
       </c>
       <c r="C291">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
@@ -3618,7 +3618,7 @@
         <v>6</v>
       </c>
       <c r="C292">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
@@ -3629,7 +3629,7 @@
         <v>6</v>
       </c>
       <c r="C293">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
@@ -3640,7 +3640,7 @@
         <v>6</v>
       </c>
       <c r="C294">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
@@ -3651,7 +3651,7 @@
         <v>6</v>
       </c>
       <c r="C295">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
@@ -3662,7 +3662,7 @@
         <v>6</v>
       </c>
       <c r="C296">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
@@ -3673,7 +3673,7 @@
         <v>6</v>
       </c>
       <c r="C297">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
@@ -3684,7 +3684,7 @@
         <v>6</v>
       </c>
       <c r="C298">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
@@ -3695,7 +3695,7 @@
         <v>6</v>
       </c>
       <c r="C299">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
@@ -3706,7 +3706,7 @@
         <v>6</v>
       </c>
       <c r="C300">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
@@ -3717,7 +3717,7 @@
         <v>6</v>
       </c>
       <c r="C301">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
@@ -3728,7 +3728,7 @@
         <v>6</v>
       </c>
       <c r="C302">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
@@ -3739,7 +3739,7 @@
         <v>6</v>
       </c>
       <c r="C303">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
@@ -3750,7 +3750,7 @@
         <v>6</v>
       </c>
       <c r="C304">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
@@ -3761,7 +3761,7 @@
         <v>6</v>
       </c>
       <c r="C305">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
@@ -3772,7 +3772,7 @@
         <v>6</v>
       </c>
       <c r="C306">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
@@ -3783,7 +3783,7 @@
         <v>6</v>
       </c>
       <c r="C307">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
@@ -3794,7 +3794,7 @@
         <v>6</v>
       </c>
       <c r="C308">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
@@ -3805,7 +3805,7 @@
         <v>6</v>
       </c>
       <c r="C309">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
@@ -3816,7 +3816,7 @@
         <v>6</v>
       </c>
       <c r="C310">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
@@ -3827,7 +3827,7 @@
         <v>6</v>
       </c>
       <c r="C311">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
@@ -3838,7 +3838,7 @@
         <v>6</v>
       </c>
       <c r="C312">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
@@ -3849,7 +3849,7 @@
         <v>6</v>
       </c>
       <c r="C313">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
@@ -3860,7 +3860,7 @@
         <v>6</v>
       </c>
       <c r="C314">
-        <v>4.4999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>